<commit_message>
Build Style of Delivery OWL
</commit_message>
<xml_diff>
--- a/StyleOfDelivery/BCIO_StyleOfDelivery.xlsx
+++ b/StyleOfDelivery/BCIO_StyleOfDelivery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisazhang/Documents/GitHub/ontologies/StyleOfDelivery/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/StyleOfDelivery/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DE9C7B-54F7-2147-A26F-79AABFFDC3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E536AE-EDB9-8045-8479-9725FB91A5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21640" yWindow="-19860" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="554">
   <si>
     <t>ID</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Elaboration</t>
-  </si>
-  <si>
-    <t>REL</t>
   </si>
   <si>
     <t>BFO entity</t>
@@ -648,9 +645,6 @@
     <t>communication process attribute</t>
   </si>
   <si>
-    <t>attribute</t>
-  </si>
-  <si>
     <t>An attribute of a communication process.</t>
   </si>
   <si>
@@ -1695,6 +1689,15 @@
   </si>
   <si>
     <t>Published</t>
+  </si>
+  <si>
+    <t>process attribute</t>
+  </si>
+  <si>
+    <t>REL 'is process attribute of'</t>
+  </si>
+  <si>
+    <t>BCIO:044131</t>
   </si>
 </sst>
 </file>
@@ -2043,11 +2046,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="R144" sqref="R144"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2081,3219 +2088,3225 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>525</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>526</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
+        <v>527</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>124</v>
+      </c>
+      <c r="H6" t="s">
+        <v>125</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P6" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>128</v>
+      </c>
+      <c r="I7" t="s">
+        <v>129</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" t="s">
-        <v>45</v>
+        <v>132</v>
       </c>
       <c r="M8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>172</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>174</v>
+      </c>
+      <c r="J9" t="s">
+        <v>175</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>178</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>179</v>
       </c>
       <c r="M10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P10" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>182</v>
+      </c>
+      <c r="J11" t="s">
+        <v>183</v>
       </c>
       <c r="M11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>186</v>
       </c>
       <c r="M12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>188</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>185</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>189</v>
+      </c>
+      <c r="H13" t="s">
+        <v>190</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P13" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>191</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>193</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>194</v>
       </c>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P14" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="M15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P15" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>198</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>199</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="M16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P16" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="I17" t="s">
-        <v>74</v>
-      </c>
-      <c r="J17" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="M17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P17" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>428</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>429</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>419</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" t="s">
-        <v>79</v>
+        <v>430</v>
+      </c>
+      <c r="I18" t="s">
+        <v>431</v>
       </c>
       <c r="J18" t="s">
-        <v>80</v>
+        <v>432</v>
       </c>
       <c r="M18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P18" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>369</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>350</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>370</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
-      </c>
-      <c r="J19" t="s">
-        <v>84</v>
+        <v>371</v>
       </c>
       <c r="M19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P19" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>348</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>349</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>350</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
-      </c>
-      <c r="J20" t="s">
-        <v>89</v>
+        <v>351</v>
       </c>
       <c r="M20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P20" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="J21" t="s">
+        <v>96</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P21" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>375</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>96</v>
+        <v>376</v>
       </c>
       <c r="J22" t="s">
-        <v>97</v>
+        <v>377</v>
       </c>
       <c r="M22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P22" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
-      </c>
-      <c r="H23" t="s">
-        <v>101</v>
-      </c>
-      <c r="I23" t="s">
-        <v>102</v>
+        <v>87</v>
+      </c>
+      <c r="J23" t="s">
+        <v>88</v>
       </c>
       <c r="M23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P23" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>551</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>203</v>
+      </c>
+      <c r="J24" t="s">
+        <v>204</v>
+      </c>
+      <c r="K24" t="s">
+        <v>19</v>
       </c>
       <c r="M24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P24" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>207</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>202</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="M25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P25" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>381</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>382</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" t="s">
-        <v>113</v>
+        <v>383</v>
+      </c>
+      <c r="J26" t="s">
+        <v>384</v>
       </c>
       <c r="M26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P26" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>468</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>469</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" t="s">
-        <v>117</v>
-      </c>
-      <c r="J27" t="s">
-        <v>118</v>
+        <v>470</v>
       </c>
       <c r="M27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P27" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>461</v>
       </c>
       <c r="B28" t="s">
-        <v>120</v>
+        <v>462</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>122</v>
+        <v>463</v>
       </c>
       <c r="M28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P28" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
         <v>20</v>
       </c>
-      <c r="D29" t="s">
-        <v>125</v>
-      </c>
-      <c r="H29" t="s">
-        <v>126</v>
+      <c r="G29" t="s">
+        <v>21</v>
       </c>
       <c r="M29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P29" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="I30" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="M30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P30" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="M31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P31" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
+        <v>63</v>
+      </c>
+      <c r="H32" t="s">
+        <v>64</v>
       </c>
       <c r="M32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P32" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>138</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="M33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P33" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" t="s">
-        <v>143</v>
+        <v>82</v>
+      </c>
+      <c r="J34" t="s">
+        <v>83</v>
       </c>
       <c r="M34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P34" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>146</v>
+        <v>99</v>
+      </c>
+      <c r="H35" t="s">
+        <v>100</v>
       </c>
       <c r="I35" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="M35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P35" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>148</v>
+        <v>305</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" t="s">
-        <v>150</v>
+        <v>306</v>
+      </c>
+      <c r="G36" t="s">
+        <v>307</v>
       </c>
       <c r="J36" t="s">
-        <v>151</v>
+        <v>308</v>
       </c>
       <c r="M36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P36" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
-      </c>
-      <c r="H37" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="M37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P37" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
-      </c>
-      <c r="I38" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="M38" t="s">
-        <v>23</v>
-      </c>
-      <c r="N38" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="P38" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="B39" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>164</v>
-      </c>
-      <c r="J39" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="M39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P39" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="C40" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="I40" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="M40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P40" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="J41" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="M41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P41" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>175</v>
-      </c>
-      <c r="J42" t="s">
-        <v>176</v>
+        <v>153</v>
+      </c>
+      <c r="H42" t="s">
+        <v>154</v>
       </c>
       <c r="M42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P42" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>177</v>
+        <v>337</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
-      </c>
-      <c r="H43" t="s">
-        <v>180</v>
+        <v>338</v>
+      </c>
+      <c r="I43" t="s">
+        <v>339</v>
+      </c>
+      <c r="J43" t="s">
+        <v>340</v>
       </c>
       <c r="M43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P43" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>232</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>233</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>183</v>
-      </c>
-      <c r="J44" t="s">
-        <v>184</v>
+        <v>234</v>
+      </c>
+      <c r="H44" t="s">
+        <v>235</v>
       </c>
       <c r="M44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P44" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>185</v>
+        <v>236</v>
       </c>
       <c r="B45" t="s">
-        <v>186</v>
+        <v>237</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>187</v>
+        <v>238</v>
+      </c>
+      <c r="J45" t="s">
+        <v>239</v>
       </c>
       <c r="M45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P45" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>188</v>
+        <v>249</v>
       </c>
       <c r="B46" t="s">
-        <v>189</v>
+        <v>250</v>
       </c>
       <c r="C46" t="s">
-        <v>186</v>
+        <v>237</v>
       </c>
       <c r="D46" t="s">
-        <v>190</v>
-      </c>
-      <c r="H46" t="s">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="M46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P46" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>192</v>
+        <v>252</v>
       </c>
       <c r="B47" t="s">
-        <v>193</v>
+        <v>253</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D47" t="s">
-        <v>194</v>
-      </c>
-      <c r="H47" t="s">
-        <v>195</v>
+        <v>254</v>
       </c>
       <c r="M47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P47" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>269</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>270</v>
       </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>271</v>
+      </c>
+      <c r="I48" t="s">
+        <v>272</v>
       </c>
       <c r="M48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P48" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="B49" t="s">
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>201</v>
+        <v>242</v>
+      </c>
+      <c r="H49" t="s">
+        <v>243</v>
       </c>
       <c r="M49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P49" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="B50" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="C50" t="s">
-        <v>204</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>205</v>
+        <v>246</v>
+      </c>
+      <c r="I50" t="s">
+        <v>247</v>
       </c>
       <c r="J50" t="s">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="M50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P50" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>256</v>
       </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D51" t="s">
-        <v>208</v>
+        <v>257</v>
+      </c>
+      <c r="H51" t="s">
+        <v>258</v>
+      </c>
+      <c r="I51" t="s">
+        <v>259</v>
+      </c>
+      <c r="J51" t="s">
+        <v>260</v>
       </c>
       <c r="M51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P51" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>267</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="C52" t="s">
-        <v>203</v>
+        <v>19</v>
       </c>
       <c r="D52" t="s">
-        <v>210</v>
+        <v>268</v>
       </c>
       <c r="M52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P52" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="B53" t="s">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="C53" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>213</v>
+        <v>263</v>
       </c>
       <c r="M53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P53" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>265</v>
       </c>
       <c r="C54" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D54" t="s">
-        <v>216</v>
+        <v>266</v>
       </c>
       <c r="M54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P54" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>279</v>
       </c>
       <c r="B55" t="s">
-        <v>218</v>
+        <v>280</v>
       </c>
       <c r="C55" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>219</v>
-      </c>
-      <c r="H55" t="s">
-        <v>220</v>
+        <v>281</v>
       </c>
       <c r="M55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P55" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>221</v>
+        <v>282</v>
       </c>
       <c r="B56" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="C56" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="H56" t="s">
-        <v>224</v>
+        <v>285</v>
       </c>
       <c r="M56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P56" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>225</v>
+        <v>136</v>
       </c>
       <c r="B57" t="s">
-        <v>226</v>
+        <v>137</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D57" t="s">
-        <v>227</v>
+        <v>139</v>
       </c>
       <c r="M57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P57" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>228</v>
+        <v>276</v>
       </c>
       <c r="B58" t="s">
-        <v>229</v>
+        <v>277</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D58" t="s">
-        <v>230</v>
+        <v>278</v>
       </c>
       <c r="M58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P58" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>231</v>
+        <v>273</v>
       </c>
       <c r="B59" t="s">
-        <v>232</v>
+        <v>274</v>
       </c>
       <c r="C59" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>233</v>
+        <v>275</v>
       </c>
       <c r="M59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P59" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="B60" t="s">
-        <v>235</v>
+        <v>324</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D60" t="s">
-        <v>236</v>
-      </c>
-      <c r="H60" t="s">
-        <v>237</v>
+        <v>325</v>
       </c>
       <c r="M60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P60" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>238</v>
+        <v>344</v>
       </c>
       <c r="B61" t="s">
-        <v>239</v>
+        <v>345</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D61" t="s">
-        <v>240</v>
-      </c>
-      <c r="J61" t="s">
-        <v>241</v>
+        <v>346</v>
+      </c>
+      <c r="I61" t="s">
+        <v>347</v>
       </c>
       <c r="M61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P61" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>242</v>
+        <v>372</v>
       </c>
       <c r="B62" t="s">
-        <v>243</v>
+        <v>373</v>
       </c>
       <c r="C62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D62" t="s">
-        <v>244</v>
-      </c>
-      <c r="H62" t="s">
-        <v>245</v>
+        <v>374</v>
       </c>
       <c r="M62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P62" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>246</v>
+        <v>133</v>
       </c>
       <c r="B63" t="s">
-        <v>247</v>
+        <v>134</v>
       </c>
       <c r="C63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D63" t="s">
-        <v>248</v>
-      </c>
-      <c r="I63" t="s">
-        <v>249</v>
-      </c>
-      <c r="J63" t="s">
-        <v>250</v>
+        <v>135</v>
       </c>
       <c r="M63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P63" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>251</v>
+        <v>400</v>
       </c>
       <c r="B64" t="s">
-        <v>252</v>
+        <v>401</v>
       </c>
       <c r="C64" t="s">
-        <v>239</v>
+        <v>19</v>
       </c>
       <c r="D64" t="s">
-        <v>253</v>
+        <v>402</v>
       </c>
       <c r="M64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P64" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>254</v>
+        <v>403</v>
       </c>
       <c r="B65" t="s">
-        <v>255</v>
+        <v>404</v>
       </c>
       <c r="C65" t="s">
-        <v>239</v>
+        <v>19</v>
       </c>
       <c r="D65" t="s">
-        <v>256</v>
+        <v>405</v>
       </c>
       <c r="M65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P65" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>257</v>
+        <v>449</v>
       </c>
       <c r="B66" t="s">
-        <v>258</v>
+        <v>450</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D66" t="s">
-        <v>259</v>
-      </c>
-      <c r="H66" t="s">
-        <v>260</v>
+        <v>451</v>
       </c>
       <c r="I66" t="s">
-        <v>261</v>
+        <v>452</v>
       </c>
       <c r="J66" t="s">
-        <v>262</v>
+        <v>453</v>
       </c>
       <c r="M66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P66" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>263</v>
+        <v>457</v>
       </c>
       <c r="B67" t="s">
-        <v>264</v>
+        <v>458</v>
       </c>
       <c r="C67" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D67" t="s">
-        <v>265</v>
+        <v>459</v>
+      </c>
+      <c r="J67" t="s">
+        <v>460</v>
       </c>
       <c r="M67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P67" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>266</v>
+        <v>486</v>
       </c>
       <c r="B68" t="s">
-        <v>267</v>
+        <v>311</v>
       </c>
       <c r="C68" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D68" t="s">
-        <v>268</v>
+        <v>487</v>
       </c>
       <c r="M68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P68" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>269</v>
+        <v>533</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>534</v>
       </c>
       <c r="C69" t="s">
-        <v>20</v>
+        <v>311</v>
       </c>
       <c r="D69" t="s">
-        <v>270</v>
+        <v>535</v>
+      </c>
+      <c r="H69" t="s">
+        <v>536</v>
       </c>
       <c r="M69" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P69" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>271</v>
+        <v>309</v>
       </c>
       <c r="B70" t="s">
-        <v>272</v>
+        <v>310</v>
       </c>
       <c r="C70" t="s">
-        <v>239</v>
+        <v>311</v>
       </c>
       <c r="D70" t="s">
-        <v>273</v>
-      </c>
-      <c r="I70" t="s">
-        <v>274</v>
+        <v>312</v>
+      </c>
+      <c r="H70" t="s">
+        <v>313</v>
       </c>
       <c r="M70" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P70" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>275</v>
+        <v>396</v>
       </c>
       <c r="B71" t="s">
-        <v>276</v>
+        <v>397</v>
       </c>
       <c r="C71" t="s">
-        <v>20</v>
+        <v>311</v>
       </c>
       <c r="D71" t="s">
-        <v>277</v>
+        <v>398</v>
+      </c>
+      <c r="H71" t="s">
+        <v>399</v>
       </c>
       <c r="M71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P71" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
       <c r="B72" t="s">
-        <v>279</v>
+        <v>320</v>
       </c>
       <c r="C72" t="s">
-        <v>139</v>
+        <v>311</v>
       </c>
       <c r="D72" t="s">
-        <v>280</v>
+        <v>321</v>
+      </c>
+      <c r="H72" t="s">
+        <v>322</v>
       </c>
       <c r="M72" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P72" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>281</v>
+        <v>478</v>
       </c>
       <c r="B73" t="s">
-        <v>282</v>
+        <v>479</v>
       </c>
       <c r="C73" t="s">
-        <v>139</v>
+        <v>311</v>
       </c>
       <c r="D73" t="s">
-        <v>283</v>
+        <v>480</v>
+      </c>
+      <c r="H73" t="s">
+        <v>481</v>
       </c>
       <c r="M73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P73" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>284</v>
+        <v>508</v>
       </c>
       <c r="B74" t="s">
-        <v>285</v>
+        <v>509</v>
       </c>
       <c r="C74" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D74" t="s">
-        <v>286</v>
-      </c>
-      <c r="H74" t="s">
-        <v>287</v>
+        <v>510</v>
+      </c>
+      <c r="J74" t="s">
+        <v>511</v>
       </c>
       <c r="M74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P74" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>288</v>
+        <v>517</v>
       </c>
       <c r="B75" t="s">
-        <v>289</v>
+        <v>518</v>
       </c>
       <c r="C75" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D75" t="s">
-        <v>290</v>
+        <v>519</v>
       </c>
       <c r="M75" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P75" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>291</v>
+        <v>23</v>
       </c>
       <c r="B76" t="s">
-        <v>292</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
+        <v>25</v>
+      </c>
+      <c r="D76" t="s">
         <v>26</v>
       </c>
-      <c r="D76" t="s">
-        <v>293</v>
-      </c>
       <c r="M76" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P76" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>294</v>
+        <v>38</v>
       </c>
       <c r="B77" t="s">
-        <v>295</v>
+        <v>39</v>
       </c>
       <c r="C77" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D77" t="s">
-        <v>296</v>
-      </c>
-      <c r="I77" t="s">
-        <v>297</v>
+        <v>40</v>
       </c>
       <c r="M77" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P77" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>298</v>
+        <v>553</v>
       </c>
       <c r="B78" t="s">
-        <v>299</v>
+        <v>45</v>
       </c>
       <c r="C78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D78" t="s">
-        <v>300</v>
-      </c>
-      <c r="J78" t="s">
-        <v>301</v>
+        <v>46</v>
       </c>
       <c r="M78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P78" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>302</v>
+        <v>47</v>
       </c>
       <c r="B79" t="s">
-        <v>303</v>
+        <v>48</v>
       </c>
       <c r="C79" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D79" t="s">
-        <v>304</v>
-      </c>
-      <c r="I79" t="s">
-        <v>305</v>
-      </c>
-      <c r="J79" t="s">
-        <v>306</v>
+        <v>49</v>
+      </c>
+      <c r="H79" t="s">
+        <v>50</v>
       </c>
       <c r="M79" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P79" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>307</v>
+        <v>70</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="C80" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D80" t="s">
-        <v>308</v>
-      </c>
-      <c r="G80" t="s">
-        <v>309</v>
+        <v>72</v>
+      </c>
+      <c r="I80" t="s">
+        <v>73</v>
       </c>
       <c r="J80" t="s">
-        <v>310</v>
+        <v>74</v>
       </c>
       <c r="M80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P80" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>311</v>
+        <v>75</v>
       </c>
       <c r="B81" t="s">
-        <v>312</v>
+        <v>76</v>
       </c>
       <c r="C81" t="s">
-        <v>313</v>
+        <v>25</v>
       </c>
       <c r="D81" t="s">
-        <v>314</v>
+        <v>77</v>
       </c>
       <c r="H81" t="s">
-        <v>315</v>
+        <v>78</v>
+      </c>
+      <c r="J81" t="s">
+        <v>79</v>
       </c>
       <c r="M81" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P81" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>316</v>
+        <v>109</v>
       </c>
       <c r="B82" t="s">
-        <v>317</v>
+        <v>110</v>
       </c>
       <c r="C82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D82" t="s">
-        <v>318</v>
-      </c>
-      <c r="I82" t="s">
-        <v>319</v>
-      </c>
-      <c r="J82" t="s">
-        <v>320</v>
+        <v>111</v>
+      </c>
+      <c r="G82" t="s">
+        <v>112</v>
       </c>
       <c r="M82" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P82" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>321</v>
+        <v>106</v>
       </c>
       <c r="B83" t="s">
-        <v>322</v>
+        <v>107</v>
       </c>
       <c r="C83" t="s">
-        <v>313</v>
+        <v>25</v>
       </c>
       <c r="D83" t="s">
-        <v>323</v>
-      </c>
-      <c r="H83" t="s">
-        <v>324</v>
+        <v>108</v>
       </c>
       <c r="M83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P83" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>325</v>
+        <v>209</v>
       </c>
       <c r="B84" t="s">
-        <v>326</v>
+        <v>210</v>
       </c>
       <c r="C84" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D84" t="s">
-        <v>327</v>
+        <v>211</v>
       </c>
       <c r="M84" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P84" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>328</v>
+        <v>212</v>
       </c>
       <c r="B85" t="s">
-        <v>329</v>
+        <v>213</v>
       </c>
       <c r="C85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D85" t="s">
-        <v>330</v>
-      </c>
-      <c r="H85" t="s">
-        <v>331</v>
+        <v>214</v>
       </c>
       <c r="M85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P85" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>332</v>
+        <v>215</v>
       </c>
       <c r="B86" t="s">
-        <v>333</v>
+        <v>216</v>
       </c>
       <c r="C86" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D86" t="s">
-        <v>334</v>
+        <v>217</v>
+      </c>
+      <c r="H86" t="s">
+        <v>218</v>
       </c>
       <c r="M86" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P86" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>335</v>
+        <v>219</v>
       </c>
       <c r="B87" t="s">
-        <v>336</v>
+        <v>220</v>
       </c>
       <c r="C87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D87" t="s">
-        <v>337</v>
+        <v>221</v>
       </c>
       <c r="H87" t="s">
-        <v>338</v>
+        <v>222</v>
       </c>
       <c r="M87" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P87" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>339</v>
+        <v>223</v>
       </c>
       <c r="B88" t="s">
-        <v>158</v>
+        <v>224</v>
       </c>
       <c r="C88" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D88" t="s">
-        <v>340</v>
-      </c>
-      <c r="I88" t="s">
-        <v>341</v>
-      </c>
-      <c r="J88" t="s">
-        <v>342</v>
+        <v>225</v>
       </c>
       <c r="M88" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P88" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>343</v>
+        <v>226</v>
       </c>
       <c r="B89" t="s">
-        <v>344</v>
+        <v>227</v>
       </c>
       <c r="C89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D89" t="s">
-        <v>345</v>
+        <v>228</v>
       </c>
       <c r="M89" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P89" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>346</v>
+        <v>229</v>
       </c>
       <c r="B90" t="s">
-        <v>347</v>
+        <v>230</v>
       </c>
       <c r="C90" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D90" t="s">
-        <v>348</v>
-      </c>
-      <c r="I90" t="s">
-        <v>349</v>
+        <v>231</v>
       </c>
       <c r="M90" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P90" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>350</v>
+        <v>286</v>
       </c>
       <c r="B91" t="s">
-        <v>351</v>
+        <v>287</v>
       </c>
       <c r="C91" t="s">
-        <v>352</v>
+        <v>25</v>
       </c>
       <c r="D91" t="s">
-        <v>353</v>
+        <v>288</v>
       </c>
       <c r="M91" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P91" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>354</v>
+        <v>289</v>
       </c>
       <c r="B92" t="s">
-        <v>355</v>
+        <v>290</v>
       </c>
       <c r="C92" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D92" t="s">
-        <v>356</v>
+        <v>291</v>
       </c>
       <c r="M92" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P92" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>357</v>
+        <v>292</v>
       </c>
       <c r="B93" t="s">
-        <v>358</v>
+        <v>293</v>
       </c>
       <c r="C93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D93" t="s">
-        <v>359</v>
+        <v>294</v>
+      </c>
+      <c r="I93" t="s">
+        <v>295</v>
       </c>
       <c r="M93" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P93" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="B94" t="s">
-        <v>361</v>
+        <v>301</v>
       </c>
       <c r="C94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D94" t="s">
-        <v>362</v>
+        <v>302</v>
+      </c>
+      <c r="I94" t="s">
+        <v>303</v>
       </c>
       <c r="J94" t="s">
-        <v>363</v>
+        <v>304</v>
       </c>
       <c r="M94" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P94" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>364</v>
+        <v>314</v>
       </c>
       <c r="B95" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="C95" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D95" t="s">
-        <v>366</v>
+        <v>316</v>
+      </c>
+      <c r="I95" t="s">
+        <v>317</v>
+      </c>
+      <c r="J95" t="s">
+        <v>318</v>
       </c>
       <c r="M95" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P95" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>367</v>
+        <v>326</v>
       </c>
       <c r="B96" t="s">
-        <v>368</v>
+        <v>327</v>
       </c>
       <c r="C96" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D96" t="s">
-        <v>369</v>
-      </c>
-      <c r="I96" t="s">
-        <v>370</v>
+        <v>328</v>
+      </c>
+      <c r="H96" t="s">
+        <v>329</v>
       </c>
       <c r="M96" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P96" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>371</v>
+        <v>330</v>
       </c>
       <c r="B97" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="C97" t="s">
-        <v>372</v>
+        <v>25</v>
       </c>
       <c r="D97" t="s">
-        <v>373</v>
+        <v>332</v>
       </c>
       <c r="M97" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P97" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
       <c r="B98" t="s">
-        <v>375</v>
+        <v>334</v>
       </c>
       <c r="C98" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D98" t="s">
-        <v>376</v>
+        <v>335</v>
+      </c>
+      <c r="H98" t="s">
+        <v>336</v>
       </c>
       <c r="M98" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P98" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>377</v>
+        <v>341</v>
       </c>
       <c r="B99" t="s">
-        <v>87</v>
+        <v>342</v>
       </c>
       <c r="C99" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D99" t="s">
-        <v>378</v>
-      </c>
-      <c r="J99" t="s">
-        <v>379</v>
+        <v>343</v>
       </c>
       <c r="M99" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P99" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>380</v>
+        <v>355</v>
       </c>
       <c r="B100" t="s">
-        <v>92</v>
+        <v>356</v>
       </c>
       <c r="C100" t="s">
-        <v>381</v>
+        <v>25</v>
       </c>
       <c r="D100" t="s">
-        <v>382</v>
+        <v>357</v>
       </c>
       <c r="M100" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P100" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>383</v>
+        <v>358</v>
       </c>
       <c r="B101" t="s">
-        <v>384</v>
+        <v>359</v>
       </c>
       <c r="C101" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D101" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="J101" t="s">
-        <v>386</v>
+        <v>361</v>
       </c>
       <c r="M101" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P101" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>387</v>
+        <v>362</v>
       </c>
       <c r="B102" t="s">
-        <v>388</v>
+        <v>363</v>
       </c>
       <c r="C102" t="s">
-        <v>372</v>
+        <v>25</v>
       </c>
       <c r="D102" t="s">
-        <v>389</v>
+        <v>364</v>
       </c>
       <c r="M102" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P102" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>390</v>
+        <v>365</v>
       </c>
       <c r="B103" t="s">
-        <v>391</v>
+        <v>366</v>
       </c>
       <c r="C103" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D103" t="s">
-        <v>392</v>
-      </c>
-      <c r="H103" t="s">
-        <v>393</v>
-      </c>
-      <c r="J103" t="s">
-        <v>394</v>
+        <v>367</v>
+      </c>
+      <c r="I103" t="s">
+        <v>368</v>
       </c>
       <c r="M103" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P103" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B104" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C104" t="s">
-        <v>351</v>
+        <v>25</v>
       </c>
       <c r="D104" t="s">
-        <v>397</v>
+        <v>390</v>
+      </c>
+      <c r="H104" t="s">
+        <v>391</v>
+      </c>
+      <c r="J104" t="s">
+        <v>392</v>
       </c>
       <c r="M104" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P104" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="B105" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="C105" t="s">
-        <v>313</v>
+        <v>25</v>
       </c>
       <c r="D105" t="s">
-        <v>400</v>
-      </c>
-      <c r="H105" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="M105" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P105" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="B106" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="C106" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D106" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="M106" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P106" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="B107" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="C107" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D107" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="M107" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P107" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>408</v>
+        <v>464</v>
       </c>
       <c r="B108" t="s">
-        <v>409</v>
+        <v>465</v>
       </c>
       <c r="C108" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D108" t="s">
-        <v>410</v>
+        <v>466</v>
+      </c>
+      <c r="I108" t="s">
+        <v>467</v>
       </c>
       <c r="M108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P108" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>411</v>
+        <v>471</v>
       </c>
       <c r="B109" t="s">
-        <v>412</v>
+        <v>472</v>
       </c>
       <c r="C109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D109" t="s">
-        <v>413</v>
+        <v>473</v>
+      </c>
+      <c r="G109" t="s">
+        <v>474</v>
       </c>
       <c r="M109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P109" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>414</v>
+        <v>475</v>
       </c>
       <c r="B110" t="s">
-        <v>415</v>
+        <v>476</v>
       </c>
       <c r="C110" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D110" t="s">
-        <v>416</v>
+        <v>477</v>
       </c>
       <c r="M110" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P110" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>417</v>
+        <v>492</v>
       </c>
       <c r="B111" t="s">
-        <v>418</v>
+        <v>493</v>
       </c>
       <c r="C111" t="s">
-        <v>351</v>
+        <v>25</v>
       </c>
       <c r="D111" t="s">
-        <v>419</v>
+        <v>494</v>
+      </c>
+      <c r="H111" t="s">
+        <v>495</v>
       </c>
       <c r="M111" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P111" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>420</v>
+        <v>496</v>
       </c>
       <c r="B112" t="s">
-        <v>421</v>
+        <v>497</v>
       </c>
       <c r="C112" t="s">
-        <v>418</v>
+        <v>25</v>
       </c>
       <c r="D112" t="s">
-        <v>422</v>
+        <v>498</v>
       </c>
       <c r="I112" t="s">
-        <v>423</v>
+        <v>499</v>
+      </c>
+      <c r="J112" t="s">
+        <v>500</v>
       </c>
       <c r="M112" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P112" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>424</v>
+        <v>501</v>
       </c>
       <c r="B113" t="s">
-        <v>425</v>
+        <v>502</v>
       </c>
       <c r="C113" t="s">
-        <v>421</v>
+        <v>25</v>
       </c>
       <c r="D113" t="s">
-        <v>426</v>
+        <v>503</v>
+      </c>
+      <c r="J113" t="s">
+        <v>504</v>
       </c>
       <c r="M113" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P113" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>427</v>
+        <v>512</v>
       </c>
       <c r="B114" t="s">
-        <v>428</v>
+        <v>513</v>
       </c>
       <c r="C114" t="s">
-        <v>421</v>
+        <v>25</v>
       </c>
       <c r="D114" t="s">
-        <v>429</v>
+        <v>514</v>
+      </c>
+      <c r="H114" t="s">
+        <v>515</v>
+      </c>
+      <c r="I114" t="s">
+        <v>516</v>
       </c>
       <c r="M114" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P114" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>430</v>
+        <v>528</v>
       </c>
       <c r="B115" t="s">
-        <v>431</v>
+        <v>529</v>
       </c>
       <c r="C115" t="s">
-        <v>421</v>
+        <v>25</v>
       </c>
       <c r="D115" t="s">
-        <v>432</v>
-      </c>
-      <c r="I115" t="s">
-        <v>433</v>
+        <v>530</v>
+      </c>
+      <c r="H115" t="s">
+        <v>531</v>
       </c>
       <c r="J115" t="s">
-        <v>434</v>
+        <v>532</v>
       </c>
       <c r="M115" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P115" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>435</v>
+        <v>537</v>
       </c>
       <c r="B116" t="s">
-        <v>436</v>
+        <v>538</v>
       </c>
       <c r="C116" t="s">
-        <v>418</v>
+        <v>25</v>
       </c>
       <c r="D116" t="s">
-        <v>437</v>
+        <v>539</v>
       </c>
       <c r="M116" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P116" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>438</v>
+        <v>543</v>
       </c>
       <c r="B117" t="s">
-        <v>439</v>
+        <v>544</v>
       </c>
       <c r="C117" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D117" t="s">
-        <v>440</v>
+        <v>545</v>
       </c>
       <c r="M117" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P117" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>441</v>
+        <v>546</v>
       </c>
       <c r="B118" t="s">
-        <v>442</v>
+        <v>547</v>
       </c>
       <c r="C118" t="s">
-        <v>203</v>
+        <v>25</v>
       </c>
       <c r="D118" t="s">
-        <v>443</v>
-      </c>
-      <c r="G118" t="s">
-        <v>444</v>
-      </c>
-      <c r="I118" t="s">
-        <v>445</v>
-      </c>
-      <c r="J118" t="s">
-        <v>446</v>
+        <v>548</v>
+      </c>
+      <c r="H118" t="s">
+        <v>549</v>
       </c>
       <c r="M118" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P118" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>447</v>
+        <v>488</v>
       </c>
       <c r="B119" t="s">
-        <v>448</v>
+        <v>489</v>
       </c>
       <c r="C119" t="s">
-        <v>203</v>
+        <v>19</v>
       </c>
       <c r="D119" t="s">
-        <v>449</v>
+        <v>490</v>
       </c>
       <c r="I119" t="s">
-        <v>450</v>
+        <v>491</v>
       </c>
       <c r="M119" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P119" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>451</v>
+        <v>540</v>
       </c>
       <c r="B120" t="s">
-        <v>452</v>
+        <v>541</v>
       </c>
       <c r="C120" t="s">
-        <v>20</v>
+        <v>202</v>
       </c>
       <c r="D120" t="s">
-        <v>453</v>
-      </c>
-      <c r="I120" t="s">
-        <v>454</v>
-      </c>
-      <c r="J120" t="s">
-        <v>455</v>
+        <v>542</v>
       </c>
       <c r="M120" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P120" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>454</v>
+      </c>
+      <c r="B121" t="s">
+        <v>455</v>
+      </c>
+      <c r="C121" t="s">
+        <v>202</v>
+      </c>
+      <c r="D121" t="s">
         <v>456</v>
       </c>
-      <c r="B121" t="s">
-        <v>457</v>
-      </c>
-      <c r="C121" t="s">
-        <v>203</v>
-      </c>
-      <c r="D121" t="s">
-        <v>458</v>
-      </c>
       <c r="M121" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P121" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="B122" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="C122" t="s">
-        <v>20</v>
+        <v>202</v>
       </c>
       <c r="D122" t="s">
-        <v>461</v>
-      </c>
-      <c r="J122" t="s">
-        <v>462</v>
+        <v>447</v>
+      </c>
+      <c r="I122" t="s">
+        <v>448</v>
       </c>
       <c r="M122" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P122" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>463</v>
+        <v>520</v>
       </c>
       <c r="B123" t="s">
-        <v>464</v>
+        <v>521</v>
       </c>
       <c r="C123" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="D123" t="s">
-        <v>465</v>
+        <v>522</v>
+      </c>
+      <c r="I123" t="s">
+        <v>523</v>
+      </c>
+      <c r="J123" t="s">
+        <v>524</v>
       </c>
       <c r="M123" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P123" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>466</v>
+        <v>439</v>
       </c>
       <c r="B124" t="s">
-        <v>467</v>
+        <v>440</v>
       </c>
       <c r="C124" t="s">
-        <v>26</v>
+        <v>202</v>
       </c>
       <c r="D124" t="s">
-        <v>468</v>
+        <v>441</v>
+      </c>
+      <c r="G124" t="s">
+        <v>442</v>
       </c>
       <c r="I124" t="s">
-        <v>469</v>
+        <v>443</v>
+      </c>
+      <c r="J124" t="s">
+        <v>444</v>
       </c>
       <c r="M124" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P124" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="B125" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="C125" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="D125" t="s">
-        <v>472</v>
+        <v>484</v>
+      </c>
+      <c r="I125" t="s">
+        <v>485</v>
       </c>
       <c r="M125" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P125" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>473</v>
+        <v>378</v>
       </c>
       <c r="B126" t="s">
-        <v>474</v>
+        <v>91</v>
       </c>
       <c r="C126" t="s">
-        <v>26</v>
+        <v>379</v>
       </c>
       <c r="D126" t="s">
-        <v>475</v>
-      </c>
-      <c r="G126" t="s">
-        <v>476</v>
+        <v>380</v>
       </c>
       <c r="M126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P126" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>477</v>
+        <v>393</v>
       </c>
       <c r="B127" t="s">
-        <v>478</v>
+        <v>394</v>
       </c>
       <c r="C127" t="s">
-        <v>26</v>
+        <v>349</v>
       </c>
       <c r="D127" t="s">
-        <v>479</v>
+        <v>395</v>
       </c>
       <c r="M127" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P127" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>480</v>
+        <v>415</v>
       </c>
       <c r="B128" t="s">
-        <v>481</v>
+        <v>416</v>
       </c>
       <c r="C128" t="s">
-        <v>313</v>
+        <v>349</v>
       </c>
       <c r="D128" t="s">
-        <v>482</v>
-      </c>
-      <c r="H128" t="s">
-        <v>483</v>
+        <v>417</v>
       </c>
       <c r="M128" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P128" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>484</v>
+        <v>418</v>
       </c>
       <c r="B129" t="s">
-        <v>485</v>
+        <v>419</v>
       </c>
       <c r="C129" t="s">
-        <v>203</v>
+        <v>416</v>
       </c>
       <c r="D129" t="s">
-        <v>486</v>
+        <v>420</v>
       </c>
       <c r="I129" t="s">
-        <v>487</v>
+        <v>421</v>
       </c>
       <c r="M129" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P129" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>488</v>
+        <v>425</v>
       </c>
       <c r="B130" t="s">
-        <v>313</v>
+        <v>426</v>
       </c>
       <c r="C130" t="s">
-        <v>20</v>
+        <v>419</v>
       </c>
       <c r="D130" t="s">
-        <v>489</v>
+        <v>427</v>
       </c>
       <c r="M130" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P130" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>490</v>
+        <v>433</v>
       </c>
       <c r="B131" t="s">
-        <v>491</v>
+        <v>434</v>
       </c>
       <c r="C131" t="s">
-        <v>20</v>
+        <v>416</v>
       </c>
       <c r="D131" t="s">
-        <v>492</v>
-      </c>
-      <c r="I131" t="s">
-        <v>493</v>
+        <v>435</v>
       </c>
       <c r="M131" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P131" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>494</v>
+        <v>385</v>
       </c>
       <c r="B132" t="s">
-        <v>495</v>
+        <v>386</v>
       </c>
       <c r="C132" t="s">
-        <v>26</v>
+        <v>370</v>
       </c>
       <c r="D132" t="s">
-        <v>496</v>
-      </c>
-      <c r="H132" t="s">
-        <v>497</v>
+        <v>387</v>
       </c>
       <c r="M132" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P132" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>498</v>
+        <v>422</v>
       </c>
       <c r="B133" t="s">
-        <v>499</v>
+        <v>423</v>
       </c>
       <c r="C133" t="s">
-        <v>26</v>
+        <v>419</v>
       </c>
       <c r="D133" t="s">
-        <v>500</v>
-      </c>
-      <c r="I133" t="s">
-        <v>501</v>
-      </c>
-      <c r="J133" t="s">
-        <v>502</v>
+        <v>424</v>
       </c>
       <c r="M133" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P133" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>503</v>
+        <v>35</v>
       </c>
       <c r="B134" t="s">
-        <v>504</v>
+        <v>36</v>
       </c>
       <c r="C134" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D134" t="s">
-        <v>505</v>
-      </c>
-      <c r="J134" t="s">
-        <v>506</v>
+        <v>37</v>
       </c>
       <c r="M134" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P134" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>507</v>
+        <v>41</v>
       </c>
       <c r="B135" t="s">
-        <v>508</v>
+        <v>42</v>
       </c>
       <c r="C135" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D135" t="s">
-        <v>509</v>
+        <v>43</v>
+      </c>
+      <c r="G135" t="s">
+        <v>44</v>
       </c>
       <c r="M135" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P135" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>510</v>
+        <v>51</v>
       </c>
       <c r="B136" t="s">
-        <v>511</v>
+        <v>52</v>
       </c>
       <c r="C136" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D136" t="s">
-        <v>512</v>
-      </c>
-      <c r="J136" t="s">
-        <v>513</v>
+        <v>54</v>
       </c>
       <c r="M136" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P136" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>514</v>
+        <v>155</v>
       </c>
       <c r="B137" t="s">
-        <v>515</v>
+        <v>156</v>
       </c>
       <c r="C137" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="D137" t="s">
-        <v>516</v>
-      </c>
-      <c r="H137" t="s">
-        <v>517</v>
+        <v>158</v>
       </c>
       <c r="I137" t="s">
-        <v>518</v>
+        <v>159</v>
       </c>
       <c r="M137" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="N137" t="s">
+        <v>160</v>
       </c>
       <c r="P137" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>519</v>
+        <v>113</v>
       </c>
       <c r="B138" t="s">
-        <v>520</v>
+        <v>19</v>
       </c>
       <c r="C138" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="D138" t="s">
-        <v>521</v>
+        <v>115</v>
+      </c>
+      <c r="G138" t="s">
+        <v>116</v>
+      </c>
+      <c r="J138" t="s">
+        <v>117</v>
       </c>
       <c r="M138" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P138" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>522</v>
+        <v>161</v>
       </c>
       <c r="B139" t="s">
-        <v>523</v>
+        <v>162</v>
       </c>
       <c r="C139" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
       <c r="D139" t="s">
-        <v>524</v>
-      </c>
-      <c r="I139" t="s">
-        <v>525</v>
+        <v>163</v>
       </c>
       <c r="J139" t="s">
-        <v>526</v>
+        <v>164</v>
       </c>
       <c r="M139" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P139" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>527</v>
+        <v>165</v>
       </c>
       <c r="B140" t="s">
-        <v>528</v>
+        <v>166</v>
       </c>
       <c r="C140" t="s">
-        <v>92</v>
+        <v>157</v>
       </c>
       <c r="D140" t="s">
-        <v>529</v>
+        <v>167</v>
+      </c>
+      <c r="I140" t="s">
+        <v>168</v>
       </c>
       <c r="M140" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P140" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>530</v>
+        <v>169</v>
       </c>
       <c r="B141" t="s">
-        <v>531</v>
+        <v>170</v>
       </c>
       <c r="C141" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="D141" t="s">
-        <v>532</v>
-      </c>
-      <c r="H141" t="s">
-        <v>533</v>
+        <v>171</v>
       </c>
       <c r="J141" t="s">
-        <v>534</v>
+        <v>164</v>
       </c>
       <c r="M141" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P141" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>535</v>
+        <v>205</v>
       </c>
       <c r="B142" t="s">
-        <v>536</v>
+        <v>120</v>
       </c>
       <c r="C142" t="s">
-        <v>313</v>
+        <v>19</v>
       </c>
       <c r="D142" t="s">
-        <v>537</v>
-      </c>
-      <c r="H142" t="s">
-        <v>538</v>
+        <v>206</v>
       </c>
       <c r="M142" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P142" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>539</v>
+        <v>296</v>
       </c>
       <c r="B143" t="s">
-        <v>540</v>
+        <v>297</v>
       </c>
       <c r="C143" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D143" t="s">
-        <v>541</v>
+        <v>298</v>
+      </c>
+      <c r="J143" t="s">
+        <v>299</v>
       </c>
       <c r="M143" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P143" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>542</v>
+        <v>352</v>
       </c>
       <c r="B144" t="s">
-        <v>543</v>
+        <v>353</v>
       </c>
       <c r="C144" t="s">
-        <v>203</v>
+        <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>544</v>
+        <v>354</v>
       </c>
       <c r="M144" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P144" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>545</v>
+        <v>436</v>
       </c>
       <c r="B145" t="s">
-        <v>546</v>
+        <v>437</v>
       </c>
       <c r="C145" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D145" t="s">
-        <v>547</v>
+        <v>438</v>
       </c>
       <c r="M145" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P145" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>548</v>
+        <v>505</v>
       </c>
       <c r="B146" t="s">
-        <v>549</v>
+        <v>506</v>
       </c>
       <c r="C146" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D146" t="s">
-        <v>550</v>
-      </c>
-      <c r="H146" t="s">
-        <v>551</v>
+        <v>507</v>
       </c>
       <c r="M146" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P146" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R146">
+    <sortCondition ref="A2:A146"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>